<commit_message>
Initial TMTC0032668_VerifyBanker_PrimaryOrNonPrimary_WhoIsPartOfTheActivityCanEditTheActivity - 30 Aug 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032668_VerifyMeetingsEventsActivitiesCreatedAsABankerInSF.xlsx
+++ b/TestData/TMTC0032668_VerifyMeetingsEventsActivitiesCreatedAsABankerInSF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575C7921-AF9F-4255-98B3-72FC4D143EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067B8D3B-1C83-41C7-8FA3-3924D44C9573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +16,6 @@
     <sheet name="Users" sheetId="2" r:id="rId1"/>
     <sheet name="Contact" sheetId="10" r:id="rId2"/>
     <sheet name="Activity" sheetId="11" r:id="rId3"/>
-    <sheet name="ActivityStartDate" sheetId="4" r:id="rId4"/>
-    <sheet name="ActivityListColumns" sheetId="16" r:id="rId5"/>
-    <sheet name="ActivityListAction" sheetId="17" r:id="rId6"/>
-    <sheet name="ActivityDetailButton" sheetId="18" r:id="rId7"/>
-    <sheet name="UpdateActivity" sheetId="19" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Users</t>
   </si>
@@ -87,64 +82,13 @@
     <t>Activity</t>
   </si>
   <si>
-    <t>ActivityStartDate</t>
-  </si>
-  <si>
-    <t>3 Months Ago</t>
-  </si>
-  <si>
     <t>Meeting Notes 1</t>
   </si>
   <si>
-    <t>Primary HL Contact</t>
-  </si>
-  <si>
-    <t>Primary Contact</t>
-  </si>
-  <si>
-    <t>ActivityListColumns</t>
-  </si>
-  <si>
-    <t>Start Date/Time</t>
-  </si>
-  <si>
-    <t>Meeting/Call Notes</t>
-  </si>
-  <si>
-    <t>ActivityListAction</t>
-  </si>
-  <si>
-    <t>View</t>
-  </si>
-  <si>
-    <t>Print</t>
-  </si>
-  <si>
-    <t>ActivityDetailButton</t>
-  </si>
-  <si>
-    <t>Cancel</t>
-  </si>
-  <si>
-    <t>Edit</t>
-  </si>
-  <si>
-    <t>Delete</t>
-  </si>
-  <si>
-    <t>Send Notification</t>
-  </si>
-  <si>
-    <t>View Report</t>
-  </si>
-  <si>
     <t>Automated Test Description Meeting</t>
   </si>
   <si>
     <t>Automated Test Subject Meeting</t>
-  </si>
-  <si>
-    <t>Updated Automated Test Subject Meeting</t>
   </si>
   <si>
     <t>Thomas Bailey</t>
@@ -242,14 +186,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -549,7 +490,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -574,10 +515,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>12</v>
@@ -588,7 +529,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -605,7 +546,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -647,7 +588,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -656,10 +597,10 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -667,10 +608,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -679,10 +620,10 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -690,10 +631,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -702,10 +643,10 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
@@ -713,10 +654,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -725,10 +666,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
@@ -739,201 +680,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="19.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DB2F0C-08E7-4C28-904C-3BF66314A132}">
-  <dimension ref="A1:A8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53DA6BCE-1CDF-488D-BB7A-6A9726A28F33}">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CFBBBF-20D8-45F6-8DD5-31DA021BBC64}">
-  <dimension ref="A1:A6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95D2294-D185-4874-A4CE-34B75A6DBCF8}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="35.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>